<commit_message>
Shared & context completed for chapter 4 & 5
</commit_message>
<xml_diff>
--- a/dataset/Analysis.xlsx
+++ b/dataset/Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sajed/PycharmProjects/Study-on-ChatGPT/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AF0D0BC-3614-774C-8C8F-AD3FAF337EAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6C0EE29-95A2-F849-B54B-57CE3B3F4F4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="760" windowWidth="27300" windowHeight="17300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1100" yWindow="760" windowWidth="27300" windowHeight="17300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall" sheetId="1" r:id="rId1"/>
@@ -21,21 +21,6 @@
     <sheet name="ch2_confidence" sheetId="3" r:id="rId6"/>
     <sheet name="ch3_confidence" sheetId="4" r:id="rId7"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v2.0" hidden="1">ch3_testing!$A$2</definedName>
-    <definedName name="_xlchart.v2.1" hidden="1">ch3_testing!$A$3</definedName>
-    <definedName name="_xlchart.v2.10" hidden="1">ch3_testing!$B$5:$J$5</definedName>
-    <definedName name="_xlchart.v2.11" hidden="1">ch3_testing!$B$6:$J$6</definedName>
-    <definedName name="_xlchart.v2.12" hidden="1">ch3_testing!$B$7:$J$7</definedName>
-    <definedName name="_xlchart.v2.2" hidden="1">ch3_testing!$A$4</definedName>
-    <definedName name="_xlchart.v2.3" hidden="1">ch3_testing!$A$5</definedName>
-    <definedName name="_xlchart.v2.4" hidden="1">ch3_testing!$A$6</definedName>
-    <definedName name="_xlchart.v2.5" hidden="1">ch3_testing!$A$7</definedName>
-    <definedName name="_xlchart.v2.6" hidden="1">ch3_testing!$B$1:$J$1</definedName>
-    <definedName name="_xlchart.v2.7" hidden="1">ch3_testing!$B$2:$J$2</definedName>
-    <definedName name="_xlchart.v2.8" hidden="1">ch3_testing!$B$3:$J$3</definedName>
-    <definedName name="_xlchart.v2.9" hidden="1">ch3_testing!$B$4:$J$4</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -5080,7 +5065,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" b="1"/>
               <a:t>Ch1 Confidence Graph </a:t>
             </a:r>
           </a:p>
@@ -5120,7 +5105,7 @@
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+        <c:grouping val="stacked"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -5247,29 +5232,11 @@
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5405,26 +5372,11 @@
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="4">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="6">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1</c:v>
@@ -5563,29 +5515,14 @@
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="7">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5605,6 +5542,7 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="163"/>
+        <c:overlap val="100"/>
         <c:axId val="916220367"/>
         <c:axId val="1418024303"/>
       </c:barChart>
@@ -5725,6 +5663,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="l"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.145956607495069"/>
+          <c:y val="0.12078904885843243"/>
+          <c:w val="0.11130418239140225"/>
+          <c:h val="0.14562909761802786"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10313,16 +10261,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>901700</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>279400</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11263,7 +11211,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="C1" sqref="C1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11742,7 +11690,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
@@ -11982,8 +11930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R23" sqref="R23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O4" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12027,29 +11975,11 @@
       <c r="B2">
         <v>3</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2">
         <v>8</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -12059,26 +11989,11 @@
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
       <c r="F3">
         <v>1</v>
       </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
       <c r="H3">
         <v>1</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -12091,29 +12006,14 @@
       <c r="B4">
         <v>3</v>
       </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4">
         <v>2</v>
       </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
       <c r="I4">
         <v>1</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>